<commit_message>
Updates on scenarios modelling
</commit_message>
<xml_diff>
--- a/data/Model_outputs.xlsx
+++ b/data/Model_outputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au566895_uni_au_dk/Documents/Mekanik/Master/Git/Master_Thesis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{EF69F93E-2181-2146-98E3-BA2BDA8433F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5F21F6A-86B3-4B49-9CE7-F24BDADAA798}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{EF69F93E-2181-2146-98E3-BA2BDA8433F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16D1FDEE-CABB-1741-9F18-CA444F4EC2E0}"/>
   <bookViews>
     <workbookView xWindow="5160" yWindow="3880" windowWidth="27240" windowHeight="16440" xr2:uid="{F3850CAA-C916-4A4A-8A8D-77C5A2B31E54}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Model</t>
   </si>
@@ -61,9 +61,6 @@
     <t>n_days</t>
   </si>
   <si>
-    <t>CO2_constraint</t>
-  </si>
-  <si>
     <t>Greenfield</t>
   </si>
   <si>
@@ -83,6 +80,12 @@
   </si>
   <si>
     <t>Ipopt</t>
+  </si>
+  <si>
+    <t>Global_CO2_constraint</t>
+  </si>
+  <si>
+    <t>2050CO2</t>
   </si>
 </sst>
 </file>
@@ -434,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DABA2C5-A2FA-DE4A-BAAE-147F9B60E8F7}">
-  <dimension ref="B1:M6"/>
+  <dimension ref="B1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -451,12 +454,12 @@
     <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -476,27 +479,30 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I1" t="s">
         <v>3</v>
       </c>
       <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
       <c r="M1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>14</v>
@@ -531,10 +537,13 @@
       <c r="M2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>14</v>
@@ -569,10 +578,13 @@
       <c r="M3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>14</v>
@@ -607,10 +619,13 @@
       <c r="M4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>14</v>
@@ -645,10 +660,13 @@
       <c r="M5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>8</v>
@@ -657,7 +675,7 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6">
         <v>114168</v>
@@ -682,6 +700,82 @@
       </c>
       <c r="M6">
         <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7">
+        <v>20451</v>
+      </c>
+      <c r="G7">
+        <v>1318</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>0.01</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>